<commit_message>
event order, change in data
</commit_message>
<xml_diff>
--- a/src/backup_files/crossedge_info.xlsx
+++ b/src/backup_files/crossedge_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serde\Documents\Github_repositories\CrossEdge\src\backup_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CA8FFC-9191-4F24-8299-DCC249DE333E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61240802-35C6-4F6A-9B9E-CDCE6239B9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="1826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4987" uniqueCount="1835">
   <si>
     <t>Grass</t>
   </si>
@@ -8309,12 +8309,39 @@
   <si>
     <t>north west area</t>
   </si>
+  <si>
+    <t>North mountain area</t>
+  </si>
+  <si>
+    <t>South forest area</t>
+  </si>
+  <si>
+    <t>Laurelite Dungeon</t>
+  </si>
+  <si>
+    <t>South area</t>
+  </si>
+  <si>
+    <t>East dungeon area</t>
+  </si>
+  <si>
+    <t>Brosstte 2</t>
+  </si>
+  <si>
+    <t>North dungeon area</t>
+  </si>
+  <si>
+    <t>Center town area</t>
+  </si>
+  <si>
+    <t>South forest islands</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8533,6 +8560,25 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="36">
@@ -9141,7 +9187,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9322,6 +9368,26 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="31" fillId="35" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="32" fillId="35" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -26401,8 +26467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37968D7-09DD-4FC5-99F9-A8A746878400}">
   <dimension ref="A1:I172"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31380,8 +31446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCD42BF-3D7B-4304-AD99-9A6B42B85E53}">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I113" sqref="I113"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="K173" sqref="K173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31394,7 +31460,7 @@
     <col min="6" max="6" width="17.5703125" style="55" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" style="55" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="55" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="54"/>
   </cols>
   <sheetData>
@@ -31433,66 +31499,66 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58">
-        <v>1</v>
-      </c>
-      <c r="B2" s="59" t="s">
+    <row r="2" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="76">
+        <v>1</v>
+      </c>
+      <c r="B2" s="77" t="s">
         <v>1587</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59" t="s">
+      <c r="F2" s="76"/>
+      <c r="G2" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="78" t="s">
         <v>1818</v>
       </c>
-      <c r="J2" s="63">
+      <c r="J2" s="80">
         <v>51</v>
       </c>
-      <c r="K2" s="61" t="s">
+      <c r="K2" s="79" t="s">
         <v>1805</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
-        <v>2</v>
-      </c>
-      <c r="B3" s="55" t="s">
+    <row r="3" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="76">
+        <v>2</v>
+      </c>
+      <c r="B3" s="77" t="s">
         <v>1588</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="55" t="s">
+      <c r="F3" s="76"/>
+      <c r="G3" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="78" t="s">
         <v>774</v>
       </c>
-      <c r="I3" s="62" t="s">
+      <c r="I3" s="81" t="s">
         <v>1824</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="80">
         <v>55</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="79" t="s">
         <v>1806</v>
       </c>
     </row>
@@ -31562,36 +31628,36 @@
       </c>
       <c r="H6" s="56"/>
     </row>
-    <row r="7" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58">
+    <row r="7" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="76">
         <v>6</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="77" t="s">
         <v>1591</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59" t="s">
+      <c r="F7" s="76"/>
+      <c r="G7" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="60" t="s">
+      <c r="H7" s="78" t="s">
         <v>1537</v>
       </c>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="79" t="s">
         <v>1819</v>
       </c>
-      <c r="J7" s="63">
+      <c r="J7" s="80">
         <v>51</v>
       </c>
-      <c r="K7" s="61" t="s">
+      <c r="K7" s="79" t="s">
         <v>1807</v>
       </c>
     </row>
@@ -31616,11 +31682,9 @@
         <v>89</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>774</v>
-      </c>
-      <c r="I8" s="62" t="s">
-        <v>1824</v>
-      </c>
+        <v>1828</v>
+      </c>
+      <c r="I8" s="62"/>
       <c r="J8" s="63"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -31689,69 +31753,67 @@
       </c>
       <c r="H11" s="56"/>
     </row>
-    <row r="12" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58">
+    <row r="12" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="76">
         <v>11</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="77" t="s">
         <v>1596</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59" t="s">
+      <c r="F12" s="76"/>
+      <c r="G12" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="H12" s="60" t="s">
+      <c r="H12" s="78" t="s">
         <v>1538</v>
       </c>
-      <c r="I12" s="62" t="s">
+      <c r="I12" s="81" t="s">
         <v>1814</v>
       </c>
-      <c r="J12" s="63">
+      <c r="J12" s="80">
         <v>52</v>
       </c>
-      <c r="K12" s="61" t="s">
+      <c r="K12" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58">
+    <row r="13" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="76">
         <v>12</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="77" t="s">
         <v>1597</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="59" t="s">
+      <c r="F13" s="76"/>
+      <c r="G13" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="60" t="s">
-        <v>774</v>
-      </c>
-      <c r="I13" s="62" t="s">
-        <v>1824</v>
-      </c>
-      <c r="J13" s="63">
+      <c r="H13" s="78" t="s">
+        <v>1828</v>
+      </c>
+      <c r="I13" s="81"/>
+      <c r="J13" s="80">
         <v>55</v>
       </c>
-      <c r="K13" s="61" t="s">
+      <c r="K13" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
@@ -31827,27 +31889,35 @@
       </c>
       <c r="J16" s="63"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="56">
+    <row r="17" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="76">
         <v>16</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="77" t="s">
         <v>1601</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="56"/>
-      <c r="G17" s="55" t="s">
+      <c r="F17" s="76"/>
+      <c r="G17" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="H17" s="57"/>
+      <c r="H17" s="78" t="s">
+        <v>1828</v>
+      </c>
+      <c r="J17" s="80">
+        <v>56</v>
+      </c>
+      <c r="K17" s="79" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="56">
@@ -31943,27 +32013,33 @@
       </c>
       <c r="J21" s="63"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="56">
+    <row r="22" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="58">
         <v>21</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="59" t="s">
         <v>1606</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="D22" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="55" t="s">
+      <c r="F22" s="58"/>
+      <c r="G22" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="57"/>
+      <c r="H22" s="60" t="s">
+        <v>817</v>
+      </c>
+      <c r="I22" s="62" t="s">
+        <v>1830</v>
+      </c>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="56">
@@ -32031,58 +32107,69 @@
       </c>
       <c r="H25" s="56"/>
     </row>
-    <row r="26" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="58">
+    <row r="26" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="76">
         <v>25</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="77" t="s">
         <v>1610</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="58"/>
-      <c r="G26" s="59" t="s">
+      <c r="F26" s="76"/>
+      <c r="G26" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="H26" s="66" t="s">
+      <c r="H26" s="78" t="s">
         <v>744</v>
       </c>
-      <c r="I26" s="62"/>
-      <c r="J26" s="63">
+      <c r="I26" s="81"/>
+      <c r="J26" s="80">
         <v>53</v>
       </c>
-      <c r="K26" s="61" t="s">
+      <c r="K26" s="79" t="s">
         <v>1805</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="56">
+    <row r="27" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="76">
         <v>26</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="77" t="s">
         <v>1611</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="55" t="s">
+      <c r="F27" s="76"/>
+      <c r="G27" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="57"/>
+      <c r="H27" s="78" t="s">
+        <v>817</v>
+      </c>
+      <c r="I27" s="81" t="s">
+        <v>1830</v>
+      </c>
+      <c r="J27" s="80">
+        <v>57</v>
+      </c>
+      <c r="K27" s="79" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="56">
@@ -32176,27 +32263,30 @@
       <c r="I31" s="62"/>
       <c r="J31" s="63"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="56">
+    <row r="32" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="58">
         <v>31</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="59" t="s">
         <v>1616</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="55" t="s">
+      <c r="D32" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="56"/>
-      <c r="G32" s="55" t="s">
+      <c r="F32" s="58"/>
+      <c r="G32" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="H32" s="56"/>
+      <c r="H32" s="60" t="s">
+        <v>1828</v>
+      </c>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="56">
@@ -32286,82 +32376,101 @@
       </c>
       <c r="H36" s="56"/>
     </row>
-    <row r="37" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="58">
+    <row r="37" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="76">
         <v>36</v>
       </c>
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="77" t="s">
         <v>1621</v>
       </c>
-      <c r="C37" s="59" t="s">
+      <c r="C37" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59" t="s">
+      <c r="D37" s="76"/>
+      <c r="E37" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="59" t="s">
+      <c r="F37" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="59" t="s">
+      <c r="G37" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="H37" s="60" t="s">
+      <c r="H37" s="78" t="s">
         <v>1539</v>
       </c>
-      <c r="I37" s="62" t="s">
+      <c r="I37" s="81" t="s">
         <v>1822</v>
       </c>
-      <c r="J37" s="63">
+      <c r="J37" s="80">
         <v>54</v>
       </c>
-      <c r="K37" s="61" t="s">
+      <c r="K37" s="79" t="s">
         <v>1806</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="56">
+    <row r="38" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="76">
         <v>37</v>
       </c>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="77" t="s">
         <v>1622</v>
       </c>
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="56"/>
-      <c r="E38" s="55" t="s">
+      <c r="D38" s="76"/>
+      <c r="E38" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="55" t="s">
+      <c r="F38" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="55" t="s">
+      <c r="G38" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="H38" s="57"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="56">
+      <c r="H38" s="78" t="s">
+        <v>841</v>
+      </c>
+      <c r="J38" s="80">
+        <v>66</v>
+      </c>
+      <c r="K38" s="79" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="76">
         <v>38</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="77" t="s">
         <v>1623</v>
       </c>
-      <c r="C39" s="55" t="s">
+      <c r="C39" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="55" t="s">
+      <c r="D39" s="76"/>
+      <c r="E39" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="55" t="s">
+      <c r="F39" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="55" t="s">
+      <c r="G39" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="H39" s="57"/>
+      <c r="H39" s="78" t="s">
+        <v>1831</v>
+      </c>
+      <c r="I39" s="81" t="s">
+        <v>1833</v>
+      </c>
+      <c r="J39" s="80">
+        <v>66</v>
+      </c>
+      <c r="K39" s="80" t="s">
+        <v>1806</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="56">
@@ -32477,36 +32586,36 @@
       </c>
       <c r="H44" s="56"/>
     </row>
-    <row r="45" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="58">
+    <row r="45" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="76">
         <v>44</v>
       </c>
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="77" t="s">
         <v>1629</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="59" t="s">
+      <c r="D45" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E45" s="59" t="s">
+      <c r="E45" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F45" s="58"/>
-      <c r="G45" s="59" t="s">
+      <c r="F45" s="76"/>
+      <c r="G45" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="H45" s="60" t="s">
+      <c r="H45" s="78" t="s">
         <v>1537</v>
       </c>
-      <c r="I45" s="61" t="s">
+      <c r="I45" s="79" t="s">
         <v>1810</v>
       </c>
-      <c r="J45" s="63">
+      <c r="J45" s="80">
         <v>51</v>
       </c>
-      <c r="K45" s="61" t="s">
+      <c r="K45" s="79" t="s">
         <v>1809</v>
       </c>
     </row>
@@ -32632,27 +32741,33 @@
       <c r="I50" s="62"/>
       <c r="J50" s="63"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="56">
+    <row r="51" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="58">
         <v>50</v>
       </c>
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="59" t="s">
         <v>1635</v>
       </c>
-      <c r="C51" s="55" t="s">
+      <c r="C51" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D51" s="55" t="s">
+      <c r="D51" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="E51" s="55" t="s">
+      <c r="E51" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="55" t="s">
+      <c r="F51" s="58"/>
+      <c r="G51" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="H51" s="57"/>
+      <c r="H51" s="60" t="s">
+        <v>817</v>
+      </c>
+      <c r="I51" s="62" t="s">
+        <v>1830</v>
+      </c>
+      <c r="J51" s="63"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="56">
@@ -32720,33 +32835,33 @@
       </c>
       <c r="H54" s="56"/>
     </row>
-    <row r="55" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="58">
+    <row r="55" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="76">
         <v>54</v>
       </c>
-      <c r="B55" s="59" t="s">
+      <c r="B55" s="77" t="s">
         <v>1639</v>
       </c>
-      <c r="C55" s="59" t="s">
+      <c r="C55" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D55" s="59" t="s">
+      <c r="D55" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E55" s="59" t="s">
+      <c r="E55" s="77" t="s">
         <v>839</v>
       </c>
-      <c r="F55" s="58"/>
-      <c r="G55" s="59" t="s">
+      <c r="F55" s="76"/>
+      <c r="G55" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="H55" s="60" t="s">
+      <c r="H55" s="78" t="s">
         <v>773</v>
       </c>
-      <c r="J55" s="63">
+      <c r="J55" s="80">
         <v>54</v>
       </c>
-      <c r="K55" s="61" t="s">
+      <c r="K55" s="79" t="s">
         <v>1823</v>
       </c>
     </row>
@@ -32819,27 +32934,33 @@
       </c>
       <c r="J58" s="63"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="56">
+    <row r="59" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="58">
         <v>58</v>
       </c>
-      <c r="B59" s="55" t="s">
+      <c r="B59" s="59" t="s">
         <v>1643</v>
       </c>
-      <c r="C59" s="55" t="s">
+      <c r="C59" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="55" t="s">
+      <c r="D59" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="E59" s="55" t="s">
+      <c r="E59" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F59" s="56"/>
-      <c r="G59" s="55" t="s">
+      <c r="F59" s="58"/>
+      <c r="G59" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="H59" s="56"/>
+      <c r="H59" s="60" t="s">
+        <v>774</v>
+      </c>
+      <c r="I59" s="62" t="s">
+        <v>1827</v>
+      </c>
+      <c r="J59" s="63"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="56">
@@ -32885,58 +33006,69 @@
       </c>
       <c r="H61" s="56"/>
     </row>
-    <row r="62" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="58">
+    <row r="62" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="76">
         <v>61</v>
       </c>
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="77" t="s">
         <v>1647</v>
       </c>
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="59" t="s">
+      <c r="D62" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="59" t="s">
+      <c r="E62" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F62" s="58"/>
-      <c r="G62" s="59" t="s">
+      <c r="F62" s="76"/>
+      <c r="G62" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="H62" s="66" t="s">
+      <c r="H62" s="78" t="s">
         <v>744</v>
       </c>
-      <c r="I62" s="62"/>
-      <c r="J62" s="63">
+      <c r="I62" s="81"/>
+      <c r="J62" s="80">
         <v>53</v>
       </c>
-      <c r="K62" s="61" t="s">
+      <c r="K62" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="56">
+    <row r="63" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="76">
         <v>62</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="77" t="s">
         <v>1648</v>
       </c>
-      <c r="C63" s="55" t="s">
+      <c r="C63" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="D63" s="55" t="s">
+      <c r="D63" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E63" s="55" t="s">
+      <c r="E63" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F63" s="56"/>
-      <c r="G63" s="55" t="s">
+      <c r="F63" s="76"/>
+      <c r="G63" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="H63" s="57"/>
+      <c r="H63" s="78" t="s">
+        <v>817</v>
+      </c>
+      <c r="I63" s="81" t="s">
+        <v>1830</v>
+      </c>
+      <c r="J63" s="80">
+        <v>57</v>
+      </c>
+      <c r="K63" s="79" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="56">
@@ -33030,27 +33162,36 @@
       <c r="I67" s="62"/>
       <c r="J67" s="63"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="56">
+    <row r="68" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="76">
         <v>67</v>
       </c>
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="77" t="s">
         <v>1653</v>
       </c>
-      <c r="C68" s="55" t="s">
+      <c r="C68" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="55" t="s">
+      <c r="D68" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E68" s="55" t="s">
+      <c r="E68" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="56"/>
-      <c r="G68" s="55" t="s">
+      <c r="F68" s="76"/>
+      <c r="G68" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="H68" s="57"/>
+      <c r="H68" s="78" t="s">
+        <v>816</v>
+      </c>
+      <c r="I68" s="81"/>
+      <c r="J68" s="80">
+        <v>56</v>
+      </c>
+      <c r="K68" s="79" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="56">
@@ -33143,34 +33284,34 @@
       </c>
       <c r="J72" s="63"/>
     </row>
-    <row r="73" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="58">
+    <row r="73" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="76">
         <v>72</v>
       </c>
-      <c r="B73" s="59" t="s">
+      <c r="B73" s="77" t="s">
         <v>1658</v>
       </c>
-      <c r="C73" s="59" t="s">
+      <c r="C73" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="59" t="s">
+      <c r="D73" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="E73" s="59" t="s">
+      <c r="E73" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F73" s="58"/>
-      <c r="G73" s="59" t="s">
+      <c r="F73" s="76"/>
+      <c r="G73" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="H73" s="60" t="s">
+      <c r="H73" s="78" t="s">
         <v>773</v>
       </c>
-      <c r="I73" s="62"/>
-      <c r="J73" s="63">
+      <c r="I73" s="81"/>
+      <c r="J73" s="80">
         <v>41</v>
       </c>
-      <c r="K73" s="61" t="s">
+      <c r="K73" s="79" t="s">
         <v>1805</v>
       </c>
     </row>
@@ -33240,60 +33381,66 @@
       </c>
       <c r="H76" s="56"/>
     </row>
-    <row r="77" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="58">
+    <row r="77" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="76">
         <v>76</v>
       </c>
-      <c r="B77" s="59" t="s">
+      <c r="B77" s="77" t="s">
         <v>1662</v>
       </c>
-      <c r="C77" s="59" t="s">
+      <c r="C77" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="D77" s="59" t="s">
+      <c r="D77" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E77" s="59" t="s">
+      <c r="E77" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F77" s="58"/>
-      <c r="G77" s="59" t="s">
+      <c r="F77" s="76"/>
+      <c r="G77" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="H77" s="60" t="s">
+      <c r="H77" s="78" t="s">
         <v>1817</v>
       </c>
-      <c r="I77" s="62" t="s">
+      <c r="I77" s="81" t="s">
         <v>1815</v>
       </c>
-      <c r="J77" s="63">
+      <c r="J77" s="80">
         <v>53</v>
       </c>
-      <c r="K77" s="61" t="s">
+      <c r="K77" s="79" t="s">
         <v>1805</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="56">
+    <row r="78" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="64">
         <v>77</v>
       </c>
-      <c r="B78" s="55" t="s">
+      <c r="B78" s="65" t="s">
         <v>1663</v>
       </c>
-      <c r="C78" s="55" t="s">
+      <c r="C78" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="55" t="s">
+      <c r="D78" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="E78" s="55" t="s">
+      <c r="E78" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="F78" s="56"/>
-      <c r="G78" s="55" t="s">
+      <c r="F78" s="64"/>
+      <c r="G78" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="H78" s="57"/>
+      <c r="H78" s="66" t="s">
+        <v>1831</v>
+      </c>
+      <c r="I78" s="62" t="s">
+        <v>1832</v>
+      </c>
+      <c r="J78" s="67"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="56">
@@ -33361,56 +33508,59 @@
       </c>
       <c r="H81" s="56"/>
     </row>
-    <row r="82" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="58">
+    <row r="82" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="76">
         <v>81</v>
       </c>
-      <c r="B82" s="59" t="s">
+      <c r="B82" s="77" t="s">
         <v>1667</v>
       </c>
-      <c r="C82" s="59" t="s">
+      <c r="C82" s="77" t="s">
         <v>154</v>
       </c>
-      <c r="D82" s="58"/>
-      <c r="E82" s="59" t="s">
+      <c r="D82" s="76"/>
+      <c r="E82" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F82" s="58"/>
-      <c r="G82" s="59" t="s">
+      <c r="F82" s="76"/>
+      <c r="G82" s="77" t="s">
         <v>154</v>
       </c>
-      <c r="H82" s="60" t="s">
+      <c r="H82" s="78" t="s">
         <v>745</v>
       </c>
-      <c r="I82" s="62"/>
-      <c r="J82" s="63">
+      <c r="I82" s="81"/>
+      <c r="J82" s="80">
         <v>52</v>
       </c>
-      <c r="K82" s="61" t="s">
+      <c r="K82" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="56">
+    <row r="83" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="58">
         <v>82</v>
       </c>
-      <c r="B83" s="55" t="s">
+      <c r="B83" s="59" t="s">
         <v>1668</v>
       </c>
-      <c r="C83" s="55" t="s">
+      <c r="C83" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="D83" s="55" t="s">
+      <c r="D83" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="E83" s="55" t="s">
+      <c r="E83" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F83" s="56"/>
-      <c r="G83" s="55" t="s">
+      <c r="F83" s="58"/>
+      <c r="G83" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="H83" s="57"/>
+      <c r="H83" s="60" t="s">
+        <v>1831</v>
+      </c>
+      <c r="J83" s="63"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="56">
@@ -33478,58 +33628,67 @@
       </c>
       <c r="H86" s="56"/>
     </row>
-    <row r="87" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="58">
+    <row r="87" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="76">
         <v>86</v>
       </c>
-      <c r="B87" s="59" t="s">
+      <c r="B87" s="77" t="s">
         <v>1673</v>
       </c>
-      <c r="C87" s="59" t="s">
+      <c r="C87" s="77" t="s">
         <v>159</v>
       </c>
-      <c r="D87" s="59" t="s">
+      <c r="D87" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E87" s="59" t="s">
+      <c r="E87" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F87" s="58"/>
-      <c r="G87" s="59" t="s">
+      <c r="F87" s="76"/>
+      <c r="G87" s="77" t="s">
         <v>159</v>
       </c>
-      <c r="H87" s="66" t="s">
+      <c r="H87" s="78" t="s">
         <v>744</v>
       </c>
-      <c r="I87" s="62"/>
-      <c r="J87" s="63">
+      <c r="I87" s="81"/>
+      <c r="J87" s="80">
         <v>53</v>
       </c>
-      <c r="K87" s="61" t="s">
+      <c r="K87" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="56">
+    <row r="88" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="76">
         <v>87</v>
       </c>
-      <c r="B88" s="55" t="s">
+      <c r="B88" s="77" t="s">
         <v>1674</v>
       </c>
-      <c r="C88" s="55" t="s">
+      <c r="C88" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="D88" s="55" t="s">
+      <c r="D88" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E88" s="55" t="s">
+      <c r="E88" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F88" s="56"/>
-      <c r="G88" s="55" t="s">
+      <c r="F88" s="76"/>
+      <c r="G88" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="H88" s="56"/>
+      <c r="H88" s="78" t="s">
+        <v>841</v>
+      </c>
+      <c r="I88" s="81"/>
+      <c r="J88" s="80">
+        <v>58</v>
+      </c>
+      <c r="K88" s="79" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="56">
@@ -33708,58 +33867,67 @@
       </c>
       <c r="H96" s="56"/>
     </row>
-    <row r="97" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="58">
+    <row r="97" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="76">
         <v>96</v>
       </c>
-      <c r="B97" s="59" t="s">
+      <c r="B97" s="77" t="s">
         <v>1683</v>
       </c>
-      <c r="C97" s="59" t="s">
+      <c r="C97" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="D97" s="59" t="s">
+      <c r="D97" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E97" s="59" t="s">
+      <c r="E97" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F97" s="58"/>
-      <c r="G97" s="59" t="s">
+      <c r="F97" s="76"/>
+      <c r="G97" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="H97" s="60" t="s">
+      <c r="H97" s="78" t="s">
         <v>1818</v>
       </c>
-      <c r="I97" s="62"/>
-      <c r="J97" s="63">
+      <c r="I97" s="81"/>
+      <c r="J97" s="80">
         <v>68</v>
       </c>
-      <c r="K97" s="61" t="s">
+      <c r="K97" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="56">
+    <row r="98" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="70">
         <v>97</v>
       </c>
-      <c r="B98" s="55" t="s">
+      <c r="B98" s="71" t="s">
         <v>1684</v>
       </c>
-      <c r="C98" s="55" t="s">
+      <c r="C98" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="D98" s="55" t="s">
+      <c r="D98" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E98" s="55" t="s">
+      <c r="E98" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="F98" s="56"/>
-      <c r="G98" s="55" t="s">
+      <c r="F98" s="70"/>
+      <c r="G98" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="H98" s="56"/>
+      <c r="H98" s="72" t="s">
+        <v>1828</v>
+      </c>
+      <c r="I98" s="75"/>
+      <c r="J98" s="74">
+        <v>68</v>
+      </c>
+      <c r="K98" s="73" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="56">
@@ -33807,56 +33975,64 @@
       </c>
       <c r="H100" s="56"/>
     </row>
-    <row r="101" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="58">
+    <row r="101" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="76">
         <v>100</v>
       </c>
-      <c r="B101" s="59" t="s">
+      <c r="B101" s="77" t="s">
         <v>1688</v>
       </c>
-      <c r="C101" s="59" t="s">
+      <c r="C101" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="D101" s="59" t="s">
+      <c r="D101" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="E101" s="59" t="s">
+      <c r="E101" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="F101" s="58"/>
-      <c r="G101" s="59" t="s">
+      <c r="F101" s="76"/>
+      <c r="G101" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="H101" s="60" t="s">
+      <c r="H101" s="78" t="s">
         <v>773</v>
       </c>
-      <c r="I101" s="62"/>
-      <c r="J101" s="63">
+      <c r="I101" s="81"/>
+      <c r="J101" s="80">
         <v>54</v>
       </c>
-      <c r="K101" s="61" t="s">
+      <c r="K101" s="79" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="56">
+    <row r="102" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="76">
         <v>101</v>
       </c>
-      <c r="B102" s="55" t="s">
+      <c r="B102" s="77" t="s">
         <v>1689</v>
       </c>
-      <c r="C102" s="55" t="s">
+      <c r="C102" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="D102" s="56"/>
-      <c r="E102" s="55" t="s">
+      <c r="D102" s="76"/>
+      <c r="E102" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F102" s="56"/>
-      <c r="G102" s="55" t="s">
+      <c r="F102" s="76"/>
+      <c r="G102" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="H102" s="57"/>
+      <c r="H102" s="78" t="s">
+        <v>841</v>
+      </c>
+      <c r="J102" s="80">
+        <v>58</v>
+      </c>
+      <c r="K102" s="79" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="56">
@@ -33904,133 +34080,161 @@
       </c>
       <c r="H104" s="56"/>
     </row>
-    <row r="105" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="58">
+    <row r="105" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="76">
         <v>104</v>
       </c>
-      <c r="B105" s="59" t="s">
+      <c r="B105" s="77" t="s">
         <v>1693</v>
       </c>
-      <c r="C105" s="59" t="s">
+      <c r="C105" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D105" s="59" t="s">
+      <c r="D105" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E105" s="59" t="s">
+      <c r="E105" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="F105" s="58"/>
-      <c r="G105" s="59" t="s">
+      <c r="F105" s="76"/>
+      <c r="G105" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H105" s="60" t="s">
+      <c r="H105" s="78" t="s">
         <v>745</v>
       </c>
-      <c r="I105" s="62"/>
-      <c r="J105" s="63">
+      <c r="I105" s="81"/>
+      <c r="J105" s="80">
         <v>70</v>
       </c>
-      <c r="K105" s="61" t="s">
+      <c r="K105" s="79" t="s">
         <v>1806</v>
       </c>
     </row>
-    <row r="106" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="58">
+    <row r="106" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="76">
         <v>105</v>
       </c>
-      <c r="B106" s="59" t="s">
+      <c r="B106" s="77" t="s">
         <v>1694</v>
       </c>
-      <c r="C106" s="59" t="s">
+      <c r="C106" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D106" s="59" t="s">
+      <c r="D106" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E106" s="59" t="s">
+      <c r="E106" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="F106" s="58"/>
-      <c r="G106" s="59" t="s">
+      <c r="F106" s="76"/>
+      <c r="G106" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H106" s="60" t="s">
+      <c r="H106" s="78" t="s">
         <v>745</v>
       </c>
-      <c r="I106" s="62"/>
-      <c r="J106" s="63">
+      <c r="I106" s="81"/>
+      <c r="J106" s="80">
         <v>71</v>
       </c>
-      <c r="K106" s="61" t="s">
+      <c r="K106" s="79" t="s">
         <v>1806</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="56">
+    <row r="107" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="76">
         <v>106</v>
       </c>
-      <c r="B107" s="55" t="s">
+      <c r="B107" s="77" t="s">
         <v>1695</v>
       </c>
-      <c r="C107" s="55" t="s">
+      <c r="C107" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D107" s="55" t="s">
+      <c r="D107" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E107" s="55" t="s">
+      <c r="E107" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="F107" s="56"/>
-      <c r="G107" s="55" t="s">
+      <c r="F107" s="76"/>
+      <c r="G107" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="H107" s="57"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="56">
+      <c r="H107" s="78" t="s">
+        <v>816</v>
+      </c>
+      <c r="J107" s="80">
+        <v>70</v>
+      </c>
+      <c r="K107" s="79" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="76">
         <v>107</v>
       </c>
-      <c r="B108" s="55" t="s">
+      <c r="B108" s="77" t="s">
         <v>1696</v>
       </c>
-      <c r="C108" s="55" t="s">
+      <c r="C108" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D108" s="55" t="s">
+      <c r="D108" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E108" s="55" t="s">
+      <c r="E108" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="F108" s="56"/>
-      <c r="G108" s="55" t="s">
+      <c r="F108" s="76"/>
+      <c r="G108" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="H108" s="57"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="56">
+      <c r="H108" s="78" t="s">
+        <v>816</v>
+      </c>
+      <c r="I108" s="81"/>
+      <c r="J108" s="80">
+        <v>71</v>
+      </c>
+      <c r="K108" s="79" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="76">
         <v>108</v>
       </c>
-      <c r="B109" s="55" t="s">
+      <c r="B109" s="77" t="s">
         <v>1697</v>
       </c>
-      <c r="C109" s="55" t="s">
+      <c r="C109" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D109" s="55" t="s">
+      <c r="D109" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E109" s="55" t="s">
+      <c r="E109" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="F109" s="56"/>
-      <c r="G109" s="55" t="s">
+      <c r="F109" s="76"/>
+      <c r="G109" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="H109" s="56"/>
+      <c r="H109" s="78" t="s">
+        <v>796</v>
+      </c>
+      <c r="I109" s="81" t="s">
+        <v>1829</v>
+      </c>
+      <c r="J109" s="80">
+        <v>70</v>
+      </c>
+      <c r="K109" s="79" t="s">
+        <v>1806</v>
+      </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="56">
@@ -34280,33 +34484,33 @@
       <c r="I120" s="62"/>
       <c r="J120" s="63"/>
     </row>
-    <row r="121" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="58">
+    <row r="121" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="76">
         <v>120</v>
       </c>
-      <c r="B121" s="59" t="s">
+      <c r="B121" s="77" t="s">
         <v>1710</v>
       </c>
-      <c r="C121" s="59" t="s">
+      <c r="C121" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="D121" s="59" t="s">
+      <c r="D121" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="E121" s="59" t="s">
+      <c r="E121" s="77" t="s">
         <v>186</v>
       </c>
-      <c r="F121" s="58"/>
-      <c r="G121" s="59" t="s">
+      <c r="F121" s="76"/>
+      <c r="G121" s="77" t="s">
         <v>186</v>
       </c>
-      <c r="H121" s="60" t="s">
+      <c r="H121" s="78" t="s">
         <v>773</v>
       </c>
-      <c r="J121" s="63">
+      <c r="J121" s="80">
         <v>54</v>
       </c>
-      <c r="K121" s="61" t="s">
+      <c r="K121" s="79" t="s">
         <v>1812</v>
       </c>
     </row>
@@ -34382,49 +34586,55 @@
       </c>
       <c r="J124" s="63"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="56">
+    <row r="125" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="58">
         <v>124</v>
       </c>
-      <c r="B125" s="55" t="s">
+      <c r="B125" s="59" t="s">
         <v>1714</v>
       </c>
-      <c r="C125" s="55" t="s">
+      <c r="C125" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="D125" s="55" t="s">
+      <c r="D125" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="E125" s="55" t="s">
+      <c r="E125" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="F125" s="56"/>
-      <c r="G125" s="55" t="s">
+      <c r="F125" s="58"/>
+      <c r="G125" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="H125" s="57"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="56">
+      <c r="H125" s="60" t="s">
+        <v>1828</v>
+      </c>
+      <c r="J125" s="63"/>
+    </row>
+    <row r="126" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="58">
         <v>125</v>
       </c>
-      <c r="B126" s="55" t="s">
+      <c r="B126" s="59" t="s">
         <v>1715</v>
       </c>
-      <c r="C126" s="55" t="s">
+      <c r="C126" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D126" s="55" t="s">
+      <c r="D126" s="59" t="s">
         <v>823</v>
       </c>
-      <c r="E126" s="55" t="s">
+      <c r="E126" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="F126" s="56"/>
-      <c r="G126" s="55" t="s">
+      <c r="F126" s="58"/>
+      <c r="G126" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="H126" s="56"/>
+      <c r="H126" s="66" t="s">
+        <v>1831</v>
+      </c>
+      <c r="J126" s="63"/>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="56">
@@ -34472,64 +34682,64 @@
       </c>
       <c r="H128" s="56"/>
     </row>
-    <row r="129" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="58">
+    <row r="129" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="76">
         <v>128</v>
       </c>
-      <c r="B129" s="59" t="s">
+      <c r="B129" s="77" t="s">
         <v>1718</v>
       </c>
-      <c r="C129" s="59" t="s">
+      <c r="C129" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="D129" s="59" t="s">
+      <c r="D129" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E129" s="59" t="s">
+      <c r="E129" s="77" t="s">
         <v>194</v>
       </c>
-      <c r="F129" s="58"/>
-      <c r="G129" s="59" t="s">
+      <c r="F129" s="76"/>
+      <c r="G129" s="77" t="s">
         <v>194</v>
       </c>
-      <c r="H129" s="60" t="s">
+      <c r="H129" s="78" t="s">
         <v>745</v>
       </c>
-      <c r="J129" s="63">
+      <c r="J129" s="80">
         <v>52</v>
       </c>
-      <c r="K129" s="61" t="s">
+      <c r="K129" s="79" t="s">
         <v>1812</v>
       </c>
     </row>
-    <row r="130" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="58">
+    <row r="130" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="76">
         <v>129</v>
       </c>
-      <c r="B130" s="59" t="s">
+      <c r="B130" s="77" t="s">
         <v>1719</v>
       </c>
-      <c r="C130" s="59" t="s">
+      <c r="C130" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="D130" s="59" t="s">
+      <c r="D130" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="E130" s="59" t="s">
+      <c r="E130" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="F130" s="58"/>
-      <c r="G130" s="59" t="s">
+      <c r="F130" s="76"/>
+      <c r="G130" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="H130" s="60" t="s">
+      <c r="H130" s="78" t="s">
         <v>773</v>
       </c>
-      <c r="I130" s="62"/>
-      <c r="J130" s="63">
+      <c r="I130" s="81"/>
+      <c r="J130" s="80">
         <v>54</v>
       </c>
-      <c r="K130" s="61" t="s">
+      <c r="K130" s="79" t="s">
         <v>1812</v>
       </c>
     </row>
@@ -34629,27 +34839,36 @@
       </c>
       <c r="J134" s="63"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="56">
+    <row r="135" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="76">
         <v>134</v>
       </c>
-      <c r="B135" s="55" t="s">
+      <c r="B135" s="77" t="s">
         <v>1724</v>
       </c>
-      <c r="C135" s="55" t="s">
+      <c r="C135" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D135" s="55" t="s">
+      <c r="D135" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E135" s="55" t="s">
+      <c r="E135" s="77" t="s">
         <v>200</v>
       </c>
-      <c r="F135" s="56"/>
-      <c r="G135" s="55" t="s">
+      <c r="F135" s="76"/>
+      <c r="G135" s="77" t="s">
         <v>200</v>
       </c>
-      <c r="H135" s="56"/>
+      <c r="H135" s="78" t="s">
+        <v>1828</v>
+      </c>
+      <c r="I135" s="81"/>
+      <c r="J135" s="80">
+        <v>55</v>
+      </c>
+      <c r="K135" s="79" t="s">
+        <v>1809</v>
+      </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="56">
@@ -34813,27 +35032,33 @@
       <c r="I142" s="69"/>
       <c r="J142" s="67"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="56">
+    <row r="143" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="58">
         <v>142</v>
       </c>
-      <c r="B143" s="55" t="s">
+      <c r="B143" s="59" t="s">
         <v>1733</v>
       </c>
-      <c r="C143" s="55" t="s">
+      <c r="C143" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="D143" s="55" t="s">
+      <c r="D143" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="E143" s="55" t="s">
+      <c r="E143" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="F143" s="56"/>
-      <c r="G143" s="55" t="s">
+      <c r="F143" s="58"/>
+      <c r="G143" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="H143" s="57"/>
+      <c r="H143" s="60" t="s">
+        <v>796</v>
+      </c>
+      <c r="I143" s="62" t="s">
+        <v>1824</v>
+      </c>
+      <c r="J143" s="63"/>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="56">
@@ -34859,7 +35084,7 @@
       </c>
       <c r="H144" s="56"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="56">
         <v>144</v>
       </c>
@@ -34881,31 +35106,39 @@
       </c>
       <c r="H145" s="56"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A146" s="56">
+    <row r="146" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="76">
         <v>145</v>
       </c>
-      <c r="B146" s="55" t="s">
+      <c r="B146" s="77" t="s">
         <v>1737</v>
       </c>
-      <c r="C146" s="55" t="s">
+      <c r="C146" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D146" s="55" t="s">
+      <c r="D146" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E146" s="55" t="s">
+      <c r="E146" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="F146" s="55" t="s">
+      <c r="F146" s="77" t="s">
         <v>768</v>
       </c>
-      <c r="G146" s="55" t="s">
+      <c r="G146" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="H146" s="56"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H146" s="78" t="s">
+        <v>816</v>
+      </c>
+      <c r="J146" s="80">
+        <v>56</v>
+      </c>
+      <c r="K146" s="79" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="56">
         <v>146</v>
       </c>
@@ -34927,7 +35160,7 @@
       </c>
       <c r="H147" s="57"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="56">
         <v>147</v>
       </c>
@@ -34951,7 +35184,7 @@
       </c>
       <c r="H148" s="56"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="56">
         <v>148</v>
       </c>
@@ -34973,31 +35206,39 @@
       </c>
       <c r="H149" s="56"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="56">
+    <row r="150" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="76">
         <v>149</v>
       </c>
-      <c r="B150" s="55" t="s">
+      <c r="B150" s="77" t="s">
         <v>1741</v>
       </c>
-      <c r="C150" s="55" t="s">
+      <c r="C150" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="D150" s="55" t="s">
+      <c r="D150" s="77" t="s">
         <v>823</v>
       </c>
-      <c r="E150" s="55" t="s">
+      <c r="E150" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="F150" s="55" t="s">
+      <c r="F150" s="77" t="s">
         <v>810</v>
       </c>
-      <c r="G150" s="55" t="s">
+      <c r="G150" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="H150" s="56"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H150" s="78" t="s">
+        <v>841</v>
+      </c>
+      <c r="J150" s="80">
+        <v>58</v>
+      </c>
+      <c r="K150" s="79" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="56">
         <v>150</v>
       </c>
@@ -35021,7 +35262,7 @@
       </c>
       <c r="H151" s="57"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="56">
         <v>151</v>
       </c>
@@ -35043,7 +35284,7 @@
       </c>
       <c r="H152" s="56"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="56">
         <v>152</v>
       </c>
@@ -35065,51 +35306,73 @@
       </c>
       <c r="H153" s="56"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A154" s="56">
+    <row r="154" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="76">
         <v>153</v>
       </c>
-      <c r="B154" s="55" t="s">
+      <c r="B154" s="77" t="s">
         <v>1746</v>
       </c>
-      <c r="C154" s="55" t="s">
+      <c r="C154" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="D154" s="55" t="s">
+      <c r="D154" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E154" s="55" t="s">
+      <c r="E154" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="F154" s="56"/>
-      <c r="G154" s="55" t="s">
+      <c r="F154" s="76"/>
+      <c r="G154" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="H154" s="56"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="56">
+      <c r="H154" s="78" t="s">
+        <v>774</v>
+      </c>
+      <c r="I154" s="81" t="s">
+        <v>1826</v>
+      </c>
+      <c r="J154" s="80">
+        <v>56</v>
+      </c>
+      <c r="K154" s="79" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="76">
         <v>154</v>
       </c>
-      <c r="B155" s="55" t="s">
+      <c r="B155" s="77" t="s">
         <v>1747</v>
       </c>
-      <c r="C155" s="55" t="s">
+      <c r="C155" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="D155" s="55" t="s">
+      <c r="D155" s="77" t="s">
         <v>823</v>
       </c>
-      <c r="E155" s="55" t="s">
+      <c r="E155" s="77" t="s">
         <v>220</v>
       </c>
-      <c r="F155" s="56"/>
-      <c r="G155" s="55" t="s">
+      <c r="F155" s="76"/>
+      <c r="G155" s="77" t="s">
         <v>220</v>
       </c>
-      <c r="H155" s="57"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H155" s="78" t="s">
+        <v>1831</v>
+      </c>
+      <c r="I155" s="81" t="s">
+        <v>1834</v>
+      </c>
+      <c r="J155" s="80">
+        <v>67</v>
+      </c>
+      <c r="K155" s="79" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="56">
         <v>155</v>
       </c>
@@ -35133,7 +35396,7 @@
       </c>
       <c r="H156" s="56"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="56">
         <v>156</v>
       </c>
@@ -35155,7 +35418,7 @@
       </c>
       <c r="H157" s="56"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="56">
         <v>157</v>
       </c>
@@ -35177,7 +35440,7 @@
       </c>
       <c r="H158" s="56"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="56">
         <v>158</v>
       </c>
@@ -35201,7 +35464,7 @@
       </c>
       <c r="H159" s="56"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="56">
         <v>159</v>
       </c>
@@ -35267,62 +35530,73 @@
       </c>
       <c r="H162" s="56"/>
     </row>
-    <row r="163" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="58">
+    <row r="163" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="76">
         <v>162</v>
       </c>
-      <c r="B163" s="59" t="s">
+      <c r="B163" s="77" t="s">
         <v>1755</v>
       </c>
-      <c r="C163" s="59" t="s">
+      <c r="C163" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="D163" s="59" t="s">
+      <c r="D163" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E163" s="59" t="s">
+      <c r="E163" s="77" t="s">
         <v>228</v>
       </c>
-      <c r="F163" s="58"/>
-      <c r="G163" s="59" t="s">
+      <c r="F163" s="76"/>
+      <c r="G163" s="77" t="s">
         <v>228</v>
       </c>
-      <c r="H163" s="60" t="s">
+      <c r="H163" s="78" t="s">
         <v>774</v>
       </c>
-      <c r="I163" s="62" t="s">
+      <c r="I163" s="81" t="s">
         <v>1825</v>
       </c>
-      <c r="J163" s="63">
+      <c r="J163" s="80">
         <v>55</v>
       </c>
-      <c r="K163" s="61" t="s">
+      <c r="K163" s="79" t="s">
         <v>1812</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164" s="56">
+    <row r="164" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="76">
         <v>163</v>
       </c>
-      <c r="B164" s="55" t="s">
+      <c r="B164" s="77" t="s">
         <v>1756</v>
       </c>
-      <c r="C164" s="55" t="s">
+      <c r="C164" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="D164" s="55" t="s">
+      <c r="D164" s="77" t="s">
         <v>823</v>
       </c>
-      <c r="E164" s="55" t="s">
+      <c r="E164" s="77" t="s">
         <v>229</v>
       </c>
-      <c r="F164" s="55" t="s">
+      <c r="F164" s="77" t="s">
         <v>861</v>
       </c>
-      <c r="G164" s="55" t="s">
+      <c r="G164" s="77" t="s">
         <v>823</v>
       </c>
-      <c r="H164" s="57"/>
+      <c r="H164" s="78" t="s">
+        <v>1831</v>
+      </c>
+      <c r="I164" s="81" t="s">
+        <v>1832</v>
+      </c>
+      <c r="J164" s="80">
+        <v>67</v>
+      </c>
+      <c r="K164" s="80" t="s">
+        <v>1809</v>
+      </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="56">
@@ -35480,49 +35754,69 @@
       </c>
       <c r="H171" s="56"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A172" s="56">
+    <row r="172" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="76">
         <v>171</v>
       </c>
-      <c r="B172" s="55" t="s">
+      <c r="B172" s="77" t="s">
         <v>1763</v>
       </c>
-      <c r="C172" s="55" t="s">
+      <c r="C172" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D172" s="55" t="s">
+      <c r="D172" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="E172" s="55" t="s">
+      <c r="E172" s="77" t="s">
         <v>237</v>
       </c>
-      <c r="F172" s="56"/>
-      <c r="G172" s="55" t="s">
+      <c r="F172" s="76"/>
+      <c r="G172" s="77" t="s">
         <v>237</v>
       </c>
-      <c r="H172" s="57"/>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="56">
+      <c r="H172" s="78" t="s">
+        <v>1828</v>
+      </c>
+      <c r="I172" s="81"/>
+      <c r="J172" s="80">
+        <v>56</v>
+      </c>
+      <c r="K172" s="79" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="70">
         <v>172</v>
       </c>
-      <c r="B173" s="55" t="s">
+      <c r="B173" s="71" t="s">
         <v>1764</v>
       </c>
-      <c r="C173" s="55" t="s">
+      <c r="C173" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="D173" s="55" t="s">
+      <c r="D173" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="E173" s="55" t="s">
+      <c r="E173" s="71" t="s">
         <v>238</v>
       </c>
-      <c r="F173" s="56"/>
-      <c r="G173" s="55" t="s">
+      <c r="F173" s="70"/>
+      <c r="G173" s="71" t="s">
         <v>238</v>
       </c>
-      <c r="H173" s="56"/>
+      <c r="H173" s="72" t="s">
+        <v>817</v>
+      </c>
+      <c r="I173" s="75" t="s">
+        <v>1830</v>
+      </c>
+      <c r="J173" s="74">
+        <v>57</v>
+      </c>
+      <c r="K173" s="73" t="s">
+        <v>1809</v>
+      </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="56">
@@ -35592,7 +35886,7 @@
       </c>
       <c r="H176" s="56"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="56">
         <v>176</v>
       </c>
@@ -35614,7 +35908,7 @@
       </c>
       <c r="H177" s="56"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="56">
         <v>177</v>
       </c>
@@ -35636,7 +35930,7 @@
       </c>
       <c r="H178" s="56"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="56">
         <v>178</v>
       </c>
@@ -35658,7 +35952,7 @@
       </c>
       <c r="H179" s="56"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="56">
         <v>179</v>
       </c>
@@ -35680,7 +35974,7 @@
       </c>
       <c r="H180" s="56"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="56">
         <v>180</v>
       </c>
@@ -35702,7 +35996,7 @@
       </c>
       <c r="H181" s="56"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="56">
         <v>181</v>
       </c>
@@ -35724,7 +36018,7 @@
       </c>
       <c r="H182" s="56"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="56">
         <v>182</v>
       </c>
@@ -35746,7 +36040,7 @@
       </c>
       <c r="H183" s="56"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="56">
         <v>183</v>
       </c>
@@ -35768,29 +36062,40 @@
       </c>
       <c r="H184" s="56"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A185" s="56">
+    <row r="185" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="76">
         <v>184</v>
       </c>
-      <c r="B185" s="55" t="s">
+      <c r="B185" s="77" t="s">
         <v>1776</v>
       </c>
-      <c r="C185" s="55" t="s">
+      <c r="C185" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D185" s="55" t="s">
+      <c r="D185" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="E185" s="55" t="s">
+      <c r="E185" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="F185" s="56"/>
-      <c r="G185" s="55" t="s">
+      <c r="F185" s="76"/>
+      <c r="G185" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="H185" s="56"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H185" s="78" t="s">
+        <v>817</v>
+      </c>
+      <c r="I185" s="81" t="s">
+        <v>1830</v>
+      </c>
+      <c r="J185" s="80">
+        <v>57</v>
+      </c>
+      <c r="K185" s="79" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="56">
         <v>185</v>
       </c>
@@ -35814,7 +36119,7 @@
       </c>
       <c r="H186" s="57"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="56">
         <v>186</v>
       </c>
@@ -35838,7 +36143,7 @@
       </c>
       <c r="H187" s="56"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="56">
         <v>187</v>
       </c>
@@ -35860,7 +36165,7 @@
       </c>
       <c r="H188" s="56"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="56">
         <v>188</v>
       </c>
@@ -35882,7 +36187,7 @@
       </c>
       <c r="H189" s="57"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="56">
         <v>189</v>
       </c>
@@ -35906,7 +36211,7 @@
       </c>
       <c r="H190" s="56"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="56">
         <v>190</v>
       </c>
@@ -35928,7 +36233,7 @@
       </c>
       <c r="H191" s="56"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="56">
         <v>191</v>
       </c>
@@ -35950,29 +36255,40 @@
       </c>
       <c r="H192" s="56"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A193" s="56">
+    <row r="193" spans="1:11" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="76">
         <v>192</v>
       </c>
-      <c r="B193" s="55" t="s">
+      <c r="B193" s="77" t="s">
         <v>1784</v>
       </c>
-      <c r="C193" s="55" t="s">
+      <c r="C193" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="D193" s="55" t="s">
+      <c r="D193" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="E193" s="55" t="s">
+      <c r="E193" s="77" t="s">
         <v>258</v>
       </c>
-      <c r="F193" s="56"/>
-      <c r="G193" s="55" t="s">
+      <c r="F193" s="76"/>
+      <c r="G193" s="77" t="s">
         <v>258</v>
       </c>
-      <c r="H193" s="57"/>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H193" s="78" t="s">
+        <v>817</v>
+      </c>
+      <c r="I193" s="81" t="s">
+        <v>1819</v>
+      </c>
+      <c r="J193" s="80">
+        <v>58</v>
+      </c>
+      <c r="K193" s="79" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="56">
         <v>193</v>
       </c>
@@ -35994,7 +36310,7 @@
       </c>
       <c r="H194" s="56"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="56">
         <v>194</v>
       </c>
@@ -36016,7 +36332,7 @@
       </c>
       <c r="H195" s="56"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="56">
         <v>195</v>
       </c>
@@ -36038,7 +36354,7 @@
       </c>
       <c r="H196" s="56"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="56">
         <v>196</v>
       </c>
@@ -36062,7 +36378,7 @@
       </c>
       <c r="H197" s="56"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="56">
         <v>197</v>
       </c>
@@ -36084,7 +36400,7 @@
       </c>
       <c r="H198" s="56"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="56">
         <v>198</v>
       </c>
@@ -36106,7 +36422,7 @@
       </c>
       <c r="H199" s="56"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="56">
         <v>199</v>
       </c>

</xml_diff>